<commit_message>
Add additional timeline data.
</commit_message>
<xml_diff>
--- a/COVID Timeline.xlsx
+++ b/COVID Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BErly\Documents\CA_COVID_TImeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E071F1F2-E3C1-462B-ACAC-AF24A09BED8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ACC424-4A91-4BD3-8ED5-84BB721F5036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7C800D0D-CC76-4362-974B-133D23204248}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="320">
   <si>
     <t>date</t>
   </si>
@@ -426,9 +426,6 @@
     <t>The Centers for Disease Control updates its guidance for coronavirus testing. The CDC now says you do not necessarily need a test if you have been in close contact with a person with a COVID-19 infection, as long as you don't show symptoms. California Governor Gavin Newsom is among those critical of the change.</t>
   </si>
   <si>
-    <t>CA adopts new reopening framework</t>
-  </si>
-  <si>
     <t>Governor Gavin Newsom announces a new framework for evaluating coronavirus activity and allowing businesses to resume operations with a color-coded system. The state is moving away from the watch list; if a county was on the watch list for increased coronavirus activity then it faced additional business restrictions.</t>
   </si>
   <si>
@@ -772,6 +769,234 @@
   </si>
   <si>
     <t>CA announces four-stage plan</t>
+  </si>
+  <si>
+    <t>NYT-CA</t>
+  </si>
+  <si>
+    <t>https://www.nytimes.com/2021/06/15/us/coronavirus-california-timeline.html</t>
+  </si>
+  <si>
+    <t>Grand Princess docks in Oakland</t>
+  </si>
+  <si>
+    <t>The Grand Princess cruise ship, which was stranded off the coast of California with coronavirus cases on board, docks at the Port of Oakland. It’s a floating symbol of America’s fear of the virus.</t>
+  </si>
+  <si>
+    <t>Four largest CA school districts close</t>
+  </si>
+  <si>
+    <t>The state’s four largest school districts — Los Angeles Unified, San Diego Unified, Fresno Unified and Long Beach Unified — announce they’ll close classrooms, as health officials in Los Angeles confirm eight more coronavirus cases in the county. District officials expect the closures to last weeks.</t>
+  </si>
+  <si>
+    <t>CA adopts new color-coded reopening framework</t>
+  </si>
+  <si>
+    <t>CA passes one million cases</t>
+  </si>
+  <si>
+    <t>California becomes the second state after Texas to reach one million known coronavirus cases.</t>
+  </si>
+  <si>
+    <t>CA passes 50,000 deaths</t>
+  </si>
+  <si>
+    <t>California surpasses 50,000 known coronavirus deaths — becoming the first state to reach that bleak milestone. It’s still far from the hardest hit relative to the size of its population.</t>
+  </si>
+  <si>
+    <t>Disneyland reopens</t>
+  </si>
+  <si>
+    <t>Disneyland reopens at 25 percent capacity.</t>
+  </si>
+  <si>
+    <t>UCA</t>
+  </si>
+  <si>
+    <t>https://covid-timeline.universityofcalifornia.edu/</t>
+  </si>
+  <si>
+    <t>UC Health begins threat assessment</t>
+  </si>
+  <si>
+    <t>Dr. Carrie L. Byington is only a few weeks into her post as executive vice president of University of California Health (UCH) when she learns about the cluster of cases of a contagious and deadly new virus halfway across the globe. A specialist in infectious diseases, Dr. Byington recognizes the potential threat. She begins gathering experts from across the UC system to advise on key areas of emergency response, preparing health systems, campus and employee operations for the possibility of an emerging pandemic.</t>
+  </si>
+  <si>
+    <t>UCHealth begins developing COVID test kits</t>
+  </si>
+  <si>
+    <t>With fewer than 500 CDC-issued test kits available to health providers across the country to diagnose the virus, the U.S. is already facing a dire testing shortage when a problem with a reagent renders many of the existing tests unusable. The University of California Health (UCH) joins labs across the country to petition the FDA to develop their own. After the agency grants emergency use authorization of in-house testing, UC’s five medical centers quickly develop and ramp up capacity. UCH becomes one of the first academic health systems in the U.S. able to test for the novel disease.</t>
+  </si>
+  <si>
+    <t>UCSF begins screening  drugs for COVID treatment</t>
+  </si>
+  <si>
+    <t>UCH</t>
+  </si>
+  <si>
+    <t>By seeking a potential cure from among dozens of drugs that have already been approved as safe for human use, the team hopes to cut years off the time it can take to develop a new therapy. By December one stands out: an anti-cancer drug that demonstrates promising results in helping some hospitalized patients recover.</t>
+  </si>
+  <si>
+    <t>UCSD study reveals loss of taste and smell</t>
+  </si>
+  <si>
+    <t>Along with fever, fatigue and shortness of breath, a UC San Diego study validates loss of smell and taste as important early signs of COVID-19 infection. The study finds people with those symptoms are 10 times more likely to have COVID-19 than any other illness, offering the first empirical evidence of the link.</t>
+  </si>
+  <si>
+    <t>UCSF begins testing nasal vaccine</t>
+  </si>
+  <si>
+    <t>A team of researchers engineers synthetic molecules that can be sprayed into the nose and mouth to prevent severe coronavirus infection. AeroNabs works by hijacking and disabling the machinery the virus uses to infect cells. It could ultimately offer a valuable extra layer of protection against COVID, even in a largely vaccinated population, and provide an easy-to-distribute way to fight COVID in countries without sufficient supply of the vaccine.</t>
+  </si>
+  <si>
+    <t>UCD opens long-COVID clinic</t>
+  </si>
+  <si>
+    <t>The clinic is one of the first to help those who suffer lingering symptoms long after acute illness has passed. Along with providing care, UC also provides research to further understand the breadth and depth of the problem; it finds that 1 in 4 people infected by COVID-19 have lingering symptoms.</t>
+  </si>
+  <si>
+    <t>CA Notify Launches</t>
+  </si>
+  <si>
+    <t>Using an app developed by Apple and Google, the program anonymously alerts users if they’ve been in contact with someone who tests positive for COVID. UC San Diego Health partners with the state to roll out CA Notify and enroll millions of Californians.</t>
+  </si>
+  <si>
+    <t>ABC10</t>
+  </si>
+  <si>
+    <t>https://www.abc10.com/article/news/health/coronavirus/covid-19-timeline-pandemic/103-03046184-ed02-498b-b6d0-795a60646c6b</t>
+  </si>
+  <si>
+    <t>Lunar New Years' events cancelled</t>
+  </si>
+  <si>
+    <t>Lunar New Years' events across the Sacramento and Central Valleys announce cancellations due to coronavirus concerns.</t>
+  </si>
+  <si>
+    <t>PPE shortage</t>
+  </si>
+  <si>
+    <t>U.S. health officials also announce a shortage in personal protective equipment.</t>
+  </si>
+  <si>
+    <t>Panic buying among consumers</t>
+  </si>
+  <si>
+    <t>People "panic buying" resulted in many Sacramento area stores running low on basic supplies.</t>
+  </si>
+  <si>
+    <t>Costco suspends free samples</t>
+  </si>
+  <si>
+    <t>Costco stops giving out free samples due to coronavirus concerns.</t>
+  </si>
+  <si>
+    <t>Jeopardy and Wheel of Fortune film without audiences</t>
+  </si>
+  <si>
+    <t>"Jeopardy!" and "Wheel of Fortune" were the first shows to forgo a studio audience while taping.</t>
+  </si>
+  <si>
+    <t>Virtual mass begins</t>
+  </si>
+  <si>
+    <t>Churches in California begin virtual mass.</t>
+  </si>
+  <si>
+    <t>California Department of Alcoholic Beverage Control announced it is now allowing restaurants to sell alcoholic drinks to go. </t>
+  </si>
+  <si>
+    <t>CA allows to-go alcohol</t>
+  </si>
+  <si>
+    <t>CA launches OnwardCA</t>
+  </si>
+  <si>
+    <t>California creates OnwardCA, which was a site designed to help people find work.</t>
+  </si>
+  <si>
+    <t>CA releases 3500 inmates</t>
+  </si>
+  <si>
+    <t>The California Department of Corrections and Rehabilitation put out a plan for roughly 3,500 inmates to be released from state prisons due to the coronavirus pandemic.</t>
+  </si>
+  <si>
+    <t>CA suspends grocery bag tax</t>
+  </si>
+  <si>
+    <t>California suspends its grocery bag tax as people are encouraged not to use reusable bags during the pandemic.</t>
+  </si>
+  <si>
+    <t>Moderna vaccinations begin in CA</t>
+  </si>
+  <si>
+    <t>Moderna vaccine arrives in California. </t>
+  </si>
+  <si>
+    <t>J+J vaccine authorized</t>
+  </si>
+  <si>
+    <t>The FDA gives emergency approval to the Johnson &amp; Johnson vaccine</t>
+  </si>
+  <si>
+    <t>CDPH reports data glitch</t>
+  </si>
+  <si>
+    <t>State officials reported the glitch caused up to 300,000 records to be backlogged, although not all of them were coronavirus cases and some could be duplicates. The problem also affected the California Reportable Disease Information Exchange, also known as CalREDIE, California Health and Human Services Secretary Dr. Mark Ghaly said.</t>
+  </si>
+  <si>
+    <t>Ballot</t>
+  </si>
+  <si>
+    <t>https://ballotpedia.org/Documenting_California%27s_path_to_recovery_from_the_coronavirus_(COVID-19)_pandemic,_2020-2021</t>
+  </si>
+  <si>
+    <t>CDOE releases school guidance</t>
+  </si>
+  <si>
+    <t>The California Department of Education released a 55-page guidance document for reopening schools to public instruction. The guidance includes temperature checks before entering schools or buses, face coverings for staff and students, and physical distancing requirements.</t>
+  </si>
+  <si>
+    <t>CA announces equity metric</t>
+  </si>
+  <si>
+    <t>Health Secretary Mark Ghaly said the state will implement what it calls an equity metric for reopening. The rule will require counties to reduce infection rates in state-defined disadvantaged communities before they can move to a less restrictive phase of reopening.</t>
+  </si>
+  <si>
+    <t>CA allows multihousehold gatherings</t>
+  </si>
+  <si>
+    <t>The state released guidelines that permit individuals from up to three households to gather privately.</t>
+  </si>
+  <si>
+    <t>The California Department of Public Health issued updated guidance for personal care service businesses that permits them to resume limited in-person operations, regardless of the risk status of their county.</t>
+  </si>
+  <si>
+    <t>CA allows pseronal care services  to reopen</t>
+  </si>
+  <si>
+    <t>Supreme Court overturns religious services restrictions</t>
+  </si>
+  <si>
+    <t>In a Feb. 5 ruling, the U.S. Supreme Court held 6-3 that the state’s ban on religious services in purple-tier counties (with the strictest mitigation rules) was unconstitutional. Justices Elena Kagan, Stephen Breyer, and Sonia Sotomayor dissented. In response to the ruling, Gov. Gavin Newsom (D) announced indoor worship services are allowed at 25% capacity in purple tier counties on Feb. 6.</t>
+  </si>
+  <si>
+    <t>Vax for the Win announced</t>
+  </si>
+  <si>
+    <t>Gov. Gavin Newsom (D) announced a vaccine incentive program called Vax for the Win on May 27. Californians ages twelve and up who have received at least one vaccine dose can participate in a drawing for $50,000, for which 30 winners will be selected, and a drawing for $1.5 million, for which ten winners will be selected. Additionally, beginning May 27, the next two million people to begin and complete their vaccination will receive a $50 prepaid card—for use online or in-stores wherever major debit cards are accepted—or grocery gift card.</t>
+  </si>
+  <si>
+    <t>Six Flags vaccine partnership starts</t>
+  </si>
+  <si>
+    <t> Gov. Gavin Newsom (D) announced the state is partnering with Six Flags to offer 50,000 free amusement park tickets to residents who receive their first or second dose of a vaccine starting June 16. </t>
+  </si>
+  <si>
+    <t>CA Comeback Plan announced</t>
+  </si>
+  <si>
+    <t>On July 13, Gov. Gavin Newsom (D) announced the passage of the California Comeback Plan. Included in the law are provisions for direct payments to California residents, and appropriations for renter assistance and small business relief programs.</t>
   </si>
 </sst>
 </file>
@@ -1130,15 +1355,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6D9AC5-03B3-472C-8251-12875DE34123}">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1156,7 +1381,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1170,7 +1395,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -1184,190 +1409,190 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43835</v>
+        <v>43831</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="C3" t="s">
         <v>231</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>257</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43841</v>
+        <v>43835</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43844</v>
+        <v>43841</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43851</v>
+        <v>43844</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43853</v>
+        <v>43851</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43856</v>
+        <v>43853</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43860</v>
+        <v>43856</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43861</v>
+        <v>43858</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>276</v>
       </c>
       <c r="C10" t="s">
         <v>232</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43863</v>
+        <v>43860</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43865</v>
+        <v>43861</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
         <v>231</v>
@@ -1376,41 +1601,41 @@
         <v>47</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43867</v>
+        <v>43863</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D13" t="s">
         <v>47</v>
       </c>
       <c r="E13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>43872</v>
+        <v>43865</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D14" t="s">
         <v>47</v>
@@ -1419,378 +1644,378 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43881</v>
+        <v>43867</v>
       </c>
       <c r="B15" t="s">
-        <v>234</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E15">
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>43884</v>
+        <v>43872</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
         <v>231</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43887</v>
+        <v>43881</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>233</v>
       </c>
       <c r="C17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E17">
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43889</v>
+        <v>43884</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E18">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>43894</v>
+        <v>43887</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
       </c>
       <c r="E19">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>43895</v>
+        <v>43888</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>278</v>
       </c>
       <c r="C20" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="D20" t="s">
-        <v>227</v>
+        <v>274</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>230</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>43900</v>
+        <v>43889</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>43901</v>
+        <v>43890</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>261</v>
       </c>
       <c r="C22" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>70</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>43901</v>
+        <v>43892</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>280</v>
       </c>
       <c r="C23" t="s">
         <v>232</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
       <c r="E23">
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>43902</v>
+        <v>43894</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D24" t="s">
         <v>47</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>43902</v>
+        <v>43895</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>228</v>
       </c>
       <c r="C25" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>226</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>72</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>43902</v>
+        <v>43896</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>282</v>
       </c>
       <c r="C26" t="s">
         <v>232</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>274</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>43905</v>
+        <v>43899</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>246</v>
       </c>
       <c r="C27" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>244</v>
       </c>
       <c r="E27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>43905</v>
+        <v>43899</v>
       </c>
       <c r="B28" t="s">
-        <v>243</v>
+        <v>284</v>
       </c>
       <c r="C28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E28">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>75</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>43905</v>
+        <v>43900</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>43906</v>
+        <v>43901</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D30" t="s">
         <v>47</v>
       </c>
       <c r="E30">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>43906</v>
+        <v>43901</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E31">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43907</v>
+        <v>43902</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D32" t="s">
         <v>47</v>
       </c>
       <c r="E32">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>43909</v>
+        <v>43902</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D33" t="s">
         <v>47</v>
@@ -1799,95 +2024,95 @@
         <v>3</v>
       </c>
       <c r="F33" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>43909</v>
+        <v>43902</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E34">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>43916</v>
+        <v>43903</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>248</v>
       </c>
       <c r="C35" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D35" t="s">
-        <v>18</v>
+        <v>244</v>
       </c>
       <c r="E35">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>36</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>43921</v>
+        <v>43905</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E36">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>43924</v>
+        <v>43905</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>242</v>
       </c>
       <c r="C37" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D37" t="s">
         <v>47</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>43925</v>
+        <v>43905</v>
       </c>
       <c r="B38" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
         <v>232</v>
@@ -1896,58 +2121,58 @@
         <v>47</v>
       </c>
       <c r="E38">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>43932</v>
+        <v>43906</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>43935</v>
+        <v>43906</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="E40">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>43936</v>
+        <v>43907</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
         <v>232</v>
@@ -1956,38 +2181,38 @@
         <v>47</v>
       </c>
       <c r="E41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F41" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>43939</v>
+        <v>43908</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>286</v>
       </c>
       <c r="C42" t="s">
         <v>232</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E42">
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>99</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>43949</v>
+        <v>43909</v>
       </c>
       <c r="B43" t="s">
-        <v>244</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
         <v>232</v>
@@ -1996,98 +2221,98 @@
         <v>47</v>
       </c>
       <c r="E43">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F43" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>43951</v>
+        <v>43909</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E44">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F44" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43952</v>
+        <v>43910</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>289</v>
       </c>
       <c r="C45" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F45" t="s">
-        <v>102</v>
+        <v>288</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>43959</v>
+        <v>43910</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>263</v>
       </c>
       <c r="C46" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D46" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F46" t="s">
-        <v>104</v>
+        <v>265</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>43976</v>
+        <v>43916</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D47" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E47">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>43977</v>
+        <v>43921</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C48" t="s">
         <v>232</v>
@@ -2096,81 +2321,81 @@
         <v>47</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>43990</v>
+        <v>43922</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>292</v>
       </c>
       <c r="C49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D49" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E49">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>110</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>44000</v>
+        <v>43923</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>290</v>
       </c>
       <c r="C50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D50" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E50">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>112</v>
+        <v>291</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>44007</v>
+        <v>43924</v>
       </c>
       <c r="B51" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F51" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>44010</v>
+        <v>43925</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D52" t="s">
         <v>47</v>
@@ -2179,335 +2404,338 @@
         <v>7</v>
       </c>
       <c r="F52" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>44012</v>
+        <v>43932</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C53" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D53" t="s">
         <v>47</v>
       </c>
       <c r="E53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F53" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>44013</v>
+        <v>43934</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>266</v>
       </c>
       <c r="C54" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D54" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E54">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F54" t="s">
-        <v>119</v>
+        <v>267</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>44022</v>
+        <v>43935</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D55" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E55">
         <v>5</v>
       </c>
       <c r="F55" t="s">
-        <v>121</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>44025</v>
+        <v>43936</v>
       </c>
       <c r="B56" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D56" t="s">
         <v>47</v>
       </c>
       <c r="E56">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F56" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>44029</v>
+        <v>43939</v>
       </c>
       <c r="B57" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="C57" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D57" t="s">
         <v>47</v>
       </c>
       <c r="E57">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F57" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>44069</v>
+        <v>43944</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
+        <v>294</v>
       </c>
       <c r="C58" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D58" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58" t="s">
-        <v>128</v>
+        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>44071</v>
+        <v>43949</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>243</v>
       </c>
       <c r="C59" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D59" t="s">
         <v>47</v>
       </c>
       <c r="E59">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>44102</v>
+        <v>43951</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D60" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E60">
         <v>5</v>
       </c>
       <c r="F60" t="s">
-        <v>132</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>44106</v>
+        <v>43952</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="C61" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D61" t="s">
-        <v>18</v>
+        <v>47</v>
+      </c>
+      <c r="E61">
+        <v>6</v>
       </c>
       <c r="F61" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>44144</v>
+        <v>43959</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D62" t="s">
         <v>47</v>
       </c>
       <c r="E62">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F62" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>44148</v>
+        <v>43976</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="C63" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D63" t="s">
         <v>47</v>
       </c>
       <c r="E63">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F63" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>44152</v>
+        <v>43977</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D64" t="s">
         <v>47</v>
       </c>
       <c r="E64">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F64" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>44154</v>
+        <v>43990</v>
       </c>
       <c r="B65" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="C65" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D65" t="s">
         <v>47</v>
       </c>
       <c r="E65">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F65" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>44156</v>
+        <v>43991</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>304</v>
       </c>
       <c r="C66" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D66" t="s">
-        <v>18</v>
+        <v>302</v>
       </c>
       <c r="E66">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F66" t="s">
-        <v>42</v>
+        <v>305</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>44167</v>
+        <v>44000</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D67" t="s">
         <v>47</v>
       </c>
       <c r="E67">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F67" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>44172</v>
+        <v>44007</v>
       </c>
       <c r="B68" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="C68" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D68" t="s">
         <v>47</v>
       </c>
       <c r="E68">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>44174</v>
+        <v>44010</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="C69" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D69" t="s">
         <v>47</v>
@@ -2516,78 +2744,78 @@
         <v>7</v>
       </c>
       <c r="F69" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>44176</v>
+        <v>44012</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="C70" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D70" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E70">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F70" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>44179</v>
+        <v>44013</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C71" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D71" t="s">
         <v>47</v>
       </c>
       <c r="E71">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F71" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>44183</v>
+        <v>44022</v>
       </c>
       <c r="B72" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="C72" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D72" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E72">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F72" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>44208</v>
+        <v>44025</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="C73" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D73" t="s">
         <v>47</v>
@@ -2596,358 +2824,358 @@
         <v>5</v>
       </c>
       <c r="F73" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>44221</v>
+        <v>44029</v>
       </c>
       <c r="B74" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="C74" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D74" t="s">
         <v>47</v>
       </c>
       <c r="E74">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F74" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>44239</v>
+        <v>44046</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>300</v>
       </c>
       <c r="C75" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D75" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E75">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F75" t="s">
-        <v>153</v>
+        <v>301</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>44269</v>
+        <v>44054</v>
       </c>
       <c r="B76" t="s">
-        <v>155</v>
+        <v>268</v>
       </c>
       <c r="C76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D76" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E76">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F76" t="s">
-        <v>156</v>
+        <v>269</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>44263</v>
+        <v>44069</v>
       </c>
       <c r="B77" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="C77" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D77" t="s">
         <v>47</v>
       </c>
       <c r="E77">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F77" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>44287</v>
+        <v>44071</v>
       </c>
       <c r="B78" t="s">
-        <v>159</v>
+        <v>250</v>
       </c>
       <c r="C78" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D78" t="s">
         <v>47</v>
       </c>
       <c r="E78">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F78" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>44311</v>
+        <v>44102</v>
       </c>
       <c r="B79" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="C79" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D79" t="s">
         <v>47</v>
       </c>
       <c r="E79">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F79" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>44286</v>
+        <v>44106</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>39</v>
       </c>
       <c r="C80" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D80" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E80">
         <v>7</v>
       </c>
       <c r="F80" t="s">
-        <v>163</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>44299</v>
+        <v>44106</v>
       </c>
       <c r="B81" t="s">
-        <v>164</v>
+        <v>306</v>
       </c>
       <c r="C81" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D81" t="s">
-        <v>47</v>
+        <v>302</v>
       </c>
       <c r="E81">
         <v>6</v>
       </c>
       <c r="F81" t="s">
-        <v>165</v>
+        <v>307</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>44304</v>
+        <v>44117</v>
       </c>
       <c r="B82" t="s">
-        <v>166</v>
+        <v>308</v>
       </c>
       <c r="C82" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D82" t="s">
-        <v>47</v>
+        <v>302</v>
       </c>
       <c r="E82">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" t="s">
-        <v>167</v>
+        <v>309</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>44308</v>
+        <v>44126</v>
       </c>
       <c r="B83" t="s">
-        <v>241</v>
+        <v>311</v>
       </c>
       <c r="C83" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D83" t="s">
-        <v>47</v>
+        <v>302</v>
       </c>
       <c r="E83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" t="s">
-        <v>168</v>
+        <v>310</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>44362</v>
+        <v>44132</v>
       </c>
       <c r="B84" t="s">
-        <v>169</v>
+        <v>270</v>
       </c>
       <c r="C84" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D84" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E84">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F84" t="s">
-        <v>170</v>
+        <v>271</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>44374</v>
+        <v>44144</v>
       </c>
       <c r="B85" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="C85" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D85" t="s">
         <v>47</v>
       </c>
       <c r="E85">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F85" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>44400</v>
+        <v>44147</v>
       </c>
       <c r="B86" t="s">
-        <v>173</v>
+        <v>272</v>
       </c>
       <c r="C86" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D86" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E86">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F86" t="s">
-        <v>174</v>
+        <v>273</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>44403</v>
+        <v>44148</v>
       </c>
       <c r="B87" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
       <c r="C87" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D87" t="s">
         <v>47</v>
       </c>
       <c r="E87">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>44404</v>
+        <v>44152</v>
       </c>
       <c r="B88" t="s">
-        <v>238</v>
+        <v>136</v>
       </c>
       <c r="C88" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D88" t="s">
         <v>47</v>
       </c>
       <c r="E88">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F88" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>44406</v>
+        <v>44154</v>
       </c>
       <c r="B89" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="C89" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D89" t="s">
         <v>47</v>
       </c>
       <c r="E89">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F89" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>44407</v>
+        <v>44156</v>
       </c>
       <c r="B90" t="s">
-        <v>180</v>
+        <v>41</v>
       </c>
       <c r="C90" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="D90" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E90">
         <v>8</v>
       </c>
       <c r="F90" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>44419</v>
+        <v>44167</v>
       </c>
       <c r="B91" t="s">
-        <v>182</v>
+        <v>140</v>
       </c>
       <c r="C91" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D91" t="s">
         <v>47</v>
@@ -2956,18 +3184,18 @@
         <v>4</v>
       </c>
       <c r="F91" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>44459</v>
+        <v>44172</v>
       </c>
       <c r="B92" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="C92" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D92" t="s">
         <v>47</v>
@@ -2976,338 +3204,338 @@
         <v>6</v>
       </c>
       <c r="F92" t="s">
-        <v>185</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>44468</v>
+        <v>44174</v>
       </c>
       <c r="B93" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="C93" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D93" t="s">
         <v>47</v>
       </c>
       <c r="E93">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F93" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>44498</v>
+        <v>44176</v>
       </c>
       <c r="B94" t="s">
-        <v>188</v>
+        <v>43</v>
       </c>
       <c r="C94" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D94" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F94" t="s">
-        <v>189</v>
+        <v>44</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>44503</v>
+        <v>44177</v>
       </c>
       <c r="B95" t="s">
-        <v>190</v>
+        <v>251</v>
       </c>
       <c r="C95" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D95" t="s">
-        <v>47</v>
+        <v>244</v>
       </c>
       <c r="E95">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F95" t="s">
-        <v>191</v>
+        <v>252</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>44505</v>
+        <v>44179</v>
       </c>
       <c r="B96" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="C96" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D96" t="s">
         <v>47</v>
       </c>
       <c r="E96">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F96" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>44526</v>
+        <v>44183</v>
       </c>
       <c r="B97" t="s">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="C97" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D97" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E97">
         <v>8</v>
       </c>
       <c r="F97" t="s">
-        <v>195</v>
+        <v>46</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>44530</v>
+        <v>44186</v>
       </c>
       <c r="B98" t="s">
-        <v>196</v>
+        <v>296</v>
       </c>
       <c r="C98" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D98" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E98">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F98" t="s">
-        <v>197</v>
+        <v>297</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>44545</v>
+        <v>44208</v>
       </c>
       <c r="B99" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
       <c r="C99" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D99" t="s">
         <v>47</v>
       </c>
       <c r="E99">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>44557</v>
+        <v>44221</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C100" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D100" t="s">
         <v>47</v>
       </c>
       <c r="E100">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F100" t="s">
-        <v>201</v>
+        <v>151</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>44565</v>
+        <v>44232</v>
       </c>
       <c r="B101" t="s">
-        <v>202</v>
+        <v>312</v>
       </c>
       <c r="C101" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D101" t="s">
-        <v>47</v>
+        <v>302</v>
       </c>
       <c r="E101">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F101" t="s">
-        <v>203</v>
+        <v>313</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>44575</v>
+        <v>44239</v>
       </c>
       <c r="B102" t="s">
-        <v>204</v>
+        <v>153</v>
       </c>
       <c r="C102" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D102" t="s">
         <v>47</v>
       </c>
       <c r="E102">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F102" t="s">
-        <v>205</v>
+        <v>152</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>44579</v>
+        <v>44251</v>
       </c>
       <c r="B103" t="s">
-        <v>206</v>
+        <v>253</v>
       </c>
       <c r="C103" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D103" t="s">
-        <v>47</v>
+        <v>244</v>
       </c>
       <c r="E103">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F103" t="s">
-        <v>207</v>
+        <v>254</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>44607</v>
+        <v>44254</v>
       </c>
       <c r="B104" t="s">
-        <v>212</v>
+        <v>298</v>
       </c>
       <c r="C104" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D104" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E104">
         <v>6</v>
       </c>
       <c r="F104" t="s">
-        <v>209</v>
+        <v>299</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>44609</v>
+        <v>44269</v>
       </c>
       <c r="B105" t="s">
-        <v>210</v>
+        <v>154</v>
       </c>
       <c r="C105" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D105" t="s">
         <v>47</v>
       </c>
       <c r="E105">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F105" t="s">
-        <v>211</v>
+        <v>155</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>44621</v>
+        <v>44263</v>
       </c>
       <c r="B106" t="s">
-        <v>208</v>
+        <v>156</v>
       </c>
       <c r="C106" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D106" t="s">
         <v>47</v>
       </c>
       <c r="E106">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F106" t="s">
-        <v>213</v>
+        <v>157</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>44652</v>
+        <v>44287</v>
       </c>
       <c r="B107" t="s">
-        <v>214</v>
+        <v>158</v>
       </c>
       <c r="C107" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D107" t="s">
         <v>47</v>
       </c>
       <c r="E107">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F107" t="s">
-        <v>215</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>44669</v>
+        <v>44301</v>
       </c>
       <c r="B108" t="s">
-        <v>216</v>
+        <v>160</v>
       </c>
       <c r="C108" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D108" t="s">
         <v>47</v>
       </c>
       <c r="E108">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F108" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>44693</v>
+        <v>44286</v>
       </c>
       <c r="B109" t="s">
-        <v>219</v>
+        <v>161</v>
       </c>
       <c r="C109" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D109" t="s">
         <v>47</v>
@@ -3316,87 +3544,747 @@
         <v>7</v>
       </c>
       <c r="F109" t="s">
-        <v>218</v>
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>44733</v>
+        <v>44299</v>
       </c>
       <c r="B110" t="s">
-        <v>220</v>
+        <v>163</v>
       </c>
       <c r="C110" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D110" t="s">
         <v>47</v>
       </c>
       <c r="E110">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F110" t="s">
-        <v>221</v>
+        <v>164</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>44985</v>
+        <v>44304</v>
       </c>
       <c r="B111" t="s">
-        <v>239</v>
+        <v>165</v>
       </c>
       <c r="C111" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D111" t="s">
         <v>47</v>
       </c>
       <c r="E111">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F111" t="s">
-        <v>222</v>
+        <v>166</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>45051</v>
+        <v>44308</v>
       </c>
       <c r="B112" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="C112" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D112" t="s">
         <v>47</v>
       </c>
       <c r="E112">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F112" t="s">
-        <v>224</v>
+        <v>167</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B113" t="s">
+        <v>255</v>
+      </c>
+      <c r="C113" t="s">
+        <v>232</v>
+      </c>
+      <c r="D113" t="s">
+        <v>244</v>
+      </c>
+      <c r="E113">
+        <v>4</v>
+      </c>
+      <c r="F113" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>44343</v>
+      </c>
+      <c r="B114" t="s">
+        <v>314</v>
+      </c>
+      <c r="C114" t="s">
+        <v>234</v>
+      </c>
+      <c r="D114" t="s">
+        <v>302</v>
+      </c>
+      <c r="E114">
+        <v>5</v>
+      </c>
+      <c r="F114" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>44362</v>
+      </c>
+      <c r="B115" t="s">
+        <v>168</v>
+      </c>
+      <c r="C115" t="s">
+        <v>231</v>
+      </c>
+      <c r="D115" t="s">
+        <v>47</v>
+      </c>
+      <c r="E115">
+        <v>9</v>
+      </c>
+      <c r="F115" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B116" t="s">
+        <v>316</v>
+      </c>
+      <c r="C116" t="s">
+        <v>234</v>
+      </c>
+      <c r="D116" t="s">
+        <v>302</v>
+      </c>
+      <c r="E116">
+        <v>3</v>
+      </c>
+      <c r="F116" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>44374</v>
+      </c>
+      <c r="B117" t="s">
+        <v>170</v>
+      </c>
+      <c r="C117" t="s">
+        <v>232</v>
+      </c>
+      <c r="D117" t="s">
+        <v>47</v>
+      </c>
+      <c r="E117">
+        <v>2</v>
+      </c>
+      <c r="F117" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>44392</v>
+      </c>
+      <c r="B118" t="s">
+        <v>318</v>
+      </c>
+      <c r="C118" t="s">
+        <v>232</v>
+      </c>
+      <c r="D118" t="s">
+        <v>302</v>
+      </c>
+      <c r="E118">
+        <v>4</v>
+      </c>
+      <c r="F118" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>44400</v>
+      </c>
+      <c r="B119" t="s">
+        <v>172</v>
+      </c>
+      <c r="C119" t="s">
+        <v>232</v>
+      </c>
+      <c r="D119" t="s">
+        <v>47</v>
+      </c>
+      <c r="E119">
+        <v>4</v>
+      </c>
+      <c r="F119" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>44403</v>
+      </c>
+      <c r="B120" t="s">
+        <v>174</v>
+      </c>
+      <c r="C120" t="s">
+        <v>234</v>
+      </c>
+      <c r="D120" t="s">
+        <v>47</v>
+      </c>
+      <c r="E120">
+        <v>6</v>
+      </c>
+      <c r="F120" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>44404</v>
+      </c>
+      <c r="B121" t="s">
+        <v>237</v>
+      </c>
+      <c r="C121" t="s">
+        <v>232</v>
+      </c>
+      <c r="D121" t="s">
+        <v>47</v>
+      </c>
+      <c r="E121">
+        <v>6</v>
+      </c>
+      <c r="F121" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>44406</v>
+      </c>
+      <c r="B122" t="s">
+        <v>177</v>
+      </c>
+      <c r="C122" t="s">
+        <v>234</v>
+      </c>
+      <c r="D122" t="s">
+        <v>47</v>
+      </c>
+      <c r="E122">
+        <v>7</v>
+      </c>
+      <c r="F122" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>44407</v>
+      </c>
+      <c r="B123" t="s">
+        <v>179</v>
+      </c>
+      <c r="C123" t="s">
+        <v>230</v>
+      </c>
+      <c r="D123" t="s">
+        <v>47</v>
+      </c>
+      <c r="E123">
+        <v>8</v>
+      </c>
+      <c r="F123" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>44419</v>
+      </c>
+      <c r="B124" t="s">
+        <v>181</v>
+      </c>
+      <c r="C124" t="s">
+        <v>234</v>
+      </c>
+      <c r="D124" t="s">
+        <v>47</v>
+      </c>
+      <c r="E124">
+        <v>4</v>
+      </c>
+      <c r="F124" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B125" t="s">
+        <v>183</v>
+      </c>
+      <c r="C125" t="s">
+        <v>234</v>
+      </c>
+      <c r="D125" t="s">
+        <v>47</v>
+      </c>
+      <c r="E125">
+        <v>6</v>
+      </c>
+      <c r="F125" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>44468</v>
+      </c>
+      <c r="B126" t="s">
+        <v>185</v>
+      </c>
+      <c r="C126" t="s">
+        <v>234</v>
+      </c>
+      <c r="D126" t="s">
+        <v>47</v>
+      </c>
+      <c r="E126">
+        <v>3</v>
+      </c>
+      <c r="F126" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>44498</v>
+      </c>
+      <c r="B127" t="s">
+        <v>187</v>
+      </c>
+      <c r="C127" t="s">
+        <v>232</v>
+      </c>
+      <c r="D127" t="s">
+        <v>47</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>44503</v>
+      </c>
+      <c r="B128" t="s">
+        <v>189</v>
+      </c>
+      <c r="C128" t="s">
+        <v>234</v>
+      </c>
+      <c r="D128" t="s">
+        <v>47</v>
+      </c>
+      <c r="E128">
+        <v>7</v>
+      </c>
+      <c r="F128" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B129" t="s">
+        <v>191</v>
+      </c>
+      <c r="C129" t="s">
+        <v>236</v>
+      </c>
+      <c r="D129" t="s">
+        <v>47</v>
+      </c>
+      <c r="E129">
+        <v>6</v>
+      </c>
+      <c r="F129" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B130" t="s">
+        <v>193</v>
+      </c>
+      <c r="C130" t="s">
+        <v>230</v>
+      </c>
+      <c r="D130" t="s">
+        <v>47</v>
+      </c>
+      <c r="E130">
+        <v>8</v>
+      </c>
+      <c r="F130" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B131" t="s">
+        <v>195</v>
+      </c>
+      <c r="C131" t="s">
+        <v>236</v>
+      </c>
+      <c r="D131" t="s">
+        <v>47</v>
+      </c>
+      <c r="E131">
+        <v>6</v>
+      </c>
+      <c r="F131" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>44545</v>
+      </c>
+      <c r="B132" t="s">
+        <v>197</v>
+      </c>
+      <c r="C132" t="s">
+        <v>232</v>
+      </c>
+      <c r="D132" t="s">
+        <v>47</v>
+      </c>
+      <c r="E132">
+        <v>6</v>
+      </c>
+      <c r="F132" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>44557</v>
+      </c>
+      <c r="B133" t="s">
+        <v>199</v>
+      </c>
+      <c r="C133" t="s">
+        <v>232</v>
+      </c>
+      <c r="D133" t="s">
+        <v>47</v>
+      </c>
+      <c r="E133">
+        <v>4</v>
+      </c>
+      <c r="F133" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>44565</v>
+      </c>
+      <c r="B134" t="s">
+        <v>201</v>
+      </c>
+      <c r="C134" t="s">
+        <v>232</v>
+      </c>
+      <c r="D134" t="s">
+        <v>47</v>
+      </c>
+      <c r="E134">
+        <v>3</v>
+      </c>
+      <c r="F134" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>44575</v>
+      </c>
+      <c r="B135" t="s">
+        <v>203</v>
+      </c>
+      <c r="C135" t="s">
+        <v>232</v>
+      </c>
+      <c r="D135" t="s">
+        <v>47</v>
+      </c>
+      <c r="E135">
+        <v>2</v>
+      </c>
+      <c r="F135" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>44579</v>
+      </c>
+      <c r="B136" t="s">
+        <v>205</v>
+      </c>
+      <c r="C136" t="s">
+        <v>235</v>
+      </c>
+      <c r="D136" t="s">
+        <v>47</v>
+      </c>
+      <c r="E136">
+        <v>7</v>
+      </c>
+      <c r="F136" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>44607</v>
+      </c>
+      <c r="B137" t="s">
+        <v>211</v>
+      </c>
+      <c r="C137" t="s">
+        <v>232</v>
+      </c>
+      <c r="D137" t="s">
+        <v>47</v>
+      </c>
+      <c r="E137">
+        <v>6</v>
+      </c>
+      <c r="F137" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B138" t="s">
+        <v>209</v>
+      </c>
+      <c r="C138" t="s">
+        <v>231</v>
+      </c>
+      <c r="D138" t="s">
+        <v>47</v>
+      </c>
+      <c r="E138">
+        <v>9</v>
+      </c>
+      <c r="F138" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B139" t="s">
+        <v>207</v>
+      </c>
+      <c r="C139" t="s">
+        <v>232</v>
+      </c>
+      <c r="D139" t="s">
+        <v>47</v>
+      </c>
+      <c r="E139">
+        <v>5</v>
+      </c>
+      <c r="F139" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B140" t="s">
+        <v>213</v>
+      </c>
+      <c r="C140" t="s">
+        <v>234</v>
+      </c>
+      <c r="D140" t="s">
+        <v>47</v>
+      </c>
+      <c r="E140">
+        <v>4</v>
+      </c>
+      <c r="F140" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>44669</v>
+      </c>
+      <c r="B141" t="s">
+        <v>215</v>
+      </c>
+      <c r="C141" t="s">
+        <v>232</v>
+      </c>
+      <c r="D141" t="s">
+        <v>47</v>
+      </c>
+      <c r="E141">
+        <v>4</v>
+      </c>
+      <c r="F141" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>44693</v>
+      </c>
+      <c r="B142" t="s">
+        <v>218</v>
+      </c>
+      <c r="C142" t="s">
+        <v>230</v>
+      </c>
+      <c r="D142" t="s">
+        <v>47</v>
+      </c>
+      <c r="E142">
+        <v>7</v>
+      </c>
+      <c r="F142" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>44733</v>
+      </c>
+      <c r="B143" t="s">
+        <v>219</v>
+      </c>
+      <c r="C143" t="s">
+        <v>234</v>
+      </c>
+      <c r="D143" t="s">
+        <v>47</v>
+      </c>
+      <c r="E143">
+        <v>7</v>
+      </c>
+      <c r="F143" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B144" t="s">
+        <v>238</v>
+      </c>
+      <c r="C144" t="s">
+        <v>231</v>
+      </c>
+      <c r="D144" t="s">
+        <v>47</v>
+      </c>
+      <c r="E144">
+        <v>10</v>
+      </c>
+      <c r="F144" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B145" t="s">
+        <v>222</v>
+      </c>
+      <c r="C145" t="s">
+        <v>231</v>
+      </c>
+      <c r="D145" t="s">
+        <v>47</v>
+      </c>
+      <c r="E145">
+        <v>8</v>
+      </c>
+      <c r="F145" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
         <v>45057</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B146" t="s">
+        <v>224</v>
+      </c>
+      <c r="C146" t="s">
+        <v>231</v>
+      </c>
+      <c r="D146" t="s">
+        <v>47</v>
+      </c>
+      <c r="E146">
+        <v>8</v>
+      </c>
+      <c r="F146" t="s">
         <v>225</v>
-      </c>
-      <c r="C113" t="s">
-        <v>232</v>
-      </c>
-      <c r="D113" t="s">
-        <v>47</v>
-      </c>
-      <c r="E113">
-        <v>8</v>
-      </c>
-      <c r="F113" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3408,10 +4296,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0E4DC4-ABC2-455B-9DCE-7C09A6B70159}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3458,10 +4346,42 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" t="s">
         <v>227</v>
       </c>
-      <c r="B6" t="s">
-        <v>228</v>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B10" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add many new user inputs!
</commit_message>
<xml_diff>
--- a/COVID Timeline.xlsx
+++ b/COVID Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BErly\Documents\CA_COVID_TImeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ACC424-4A91-4BD3-8ED5-84BB721F5036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB0006-4808-4228-A100-E9D3B5D466BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7C800D0D-CC76-4362-974B-133D23204248}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{7C800D0D-CC76-4362-974B-133D23204248}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="324">
   <si>
     <t>date</t>
   </si>
@@ -997,6 +997,18 @@
   </si>
   <si>
     <t>On July 13, Gov. Gavin Newsom (D) announced the passage of the California Comeback Plan. Included in the law are provisions for direct payments to California residents, and appropriations for renter assistance and small business relief programs.</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>Timeline provided in private communicaton from Raymundo, Trudy@CDPH</t>
+  </si>
+  <si>
+    <t>Unified Support Teams develpoed</t>
+  </si>
+  <si>
+    <t>Governor Gavin Newsom announced a call to action to slow the spread of COVID-19 in these hard-hit communities. On Tuesday, July 28, 2020, the California Governor’s Office of Emergency Services (Cal OES) and the California Health and Human Services Agency (CHHS) responded by establishing the Central Valley Task Force.</t>
   </si>
 </sst>
 </file>
@@ -1355,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6D9AC5-03B3-472C-8251-12875DE34123}">
-  <dimension ref="A1:F146"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,122 +2861,122 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>44046</v>
+        <v>44040</v>
       </c>
       <c r="B75" t="s">
-        <v>300</v>
+        <v>322</v>
       </c>
       <c r="C75" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D75" t="s">
-        <v>274</v>
+        <v>320</v>
       </c>
       <c r="E75">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>44054</v>
+        <v>44046</v>
       </c>
       <c r="B76" t="s">
-        <v>268</v>
+        <v>300</v>
       </c>
       <c r="C76" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D76" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="E76">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>269</v>
+        <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>44069</v>
+        <v>44054</v>
       </c>
       <c r="B77" t="s">
-        <v>127</v>
+        <v>268</v>
       </c>
       <c r="C77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D77" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E77">
         <v>4</v>
       </c>
       <c r="F77" t="s">
-        <v>128</v>
+        <v>269</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>44071</v>
+        <v>44069</v>
       </c>
       <c r="B78" t="s">
-        <v>250</v>
+        <v>127</v>
       </c>
       <c r="C78" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D78" t="s">
         <v>47</v>
       </c>
       <c r="E78">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>44102</v>
+        <v>44071</v>
       </c>
       <c r="B79" t="s">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="C79" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D79" t="s">
         <v>47</v>
       </c>
       <c r="E79">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F79" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>44106</v>
+        <v>44102</v>
       </c>
       <c r="B80" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="C80" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D80" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E80">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F80" t="s">
-        <v>40</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2972,27 +2984,27 @@
         <v>44106</v>
       </c>
       <c r="B81" t="s">
-        <v>306</v>
+        <v>39</v>
       </c>
       <c r="C81" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D81" t="s">
-        <v>302</v>
+        <v>18</v>
       </c>
       <c r="E81">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F81" t="s">
-        <v>307</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>44117</v>
+        <v>44106</v>
       </c>
       <c r="B82" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C82" t="s">
         <v>232</v>
@@ -3004,15 +3016,15 @@
         <v>6</v>
       </c>
       <c r="F82" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>44126</v>
+        <v>44117</v>
       </c>
       <c r="B83" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C83" t="s">
         <v>232</v>
@@ -3021,178 +3033,178 @@
         <v>302</v>
       </c>
       <c r="E83">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F83" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>44132</v>
+        <v>44126</v>
       </c>
       <c r="B84" t="s">
-        <v>270</v>
+        <v>311</v>
       </c>
       <c r="C84" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D84" t="s">
-        <v>264</v>
+        <v>302</v>
       </c>
       <c r="E84">
         <v>5</v>
       </c>
       <c r="F84" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>44144</v>
+        <v>44132</v>
       </c>
       <c r="B85" t="s">
-        <v>132</v>
+        <v>270</v>
       </c>
       <c r="C85" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D85" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E85">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F85" t="s">
-        <v>133</v>
+        <v>271</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>44147</v>
+        <v>44144</v>
       </c>
       <c r="B86" t="s">
-        <v>272</v>
+        <v>132</v>
       </c>
       <c r="C86" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D86" t="s">
-        <v>264</v>
+        <v>47</v>
       </c>
       <c r="E86">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F86" t="s">
-        <v>273</v>
+        <v>133</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>44148</v>
+        <v>44147</v>
       </c>
       <c r="B87" t="s">
-        <v>134</v>
+        <v>272</v>
       </c>
       <c r="C87" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D87" t="s">
-        <v>47</v>
+        <v>264</v>
       </c>
       <c r="E87">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F87" t="s">
-        <v>135</v>
+        <v>273</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>44152</v>
+        <v>44148</v>
       </c>
       <c r="B88" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C88" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D88" t="s">
         <v>47</v>
       </c>
       <c r="E88">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F88" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>44154</v>
+        <v>44152</v>
       </c>
       <c r="B89" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C89" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D89" t="s">
         <v>47</v>
       </c>
       <c r="E89">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F89" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>44156</v>
+        <v>44154</v>
       </c>
       <c r="B90" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="C90" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D90" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E90">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F90" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>44167</v>
+        <v>44156</v>
       </c>
       <c r="B91" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="C91" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D91" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E91">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F91" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>44172</v>
+        <v>44167</v>
       </c>
       <c r="B92" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C92" t="s">
         <v>232</v>
@@ -3201,18 +3213,18 @@
         <v>47</v>
       </c>
       <c r="E92">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F92" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>44174</v>
+        <v>44172</v>
       </c>
       <c r="B93" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C93" t="s">
         <v>232</v>
@@ -3221,298 +3233,298 @@
         <v>47</v>
       </c>
       <c r="E93">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>44176</v>
+        <v>44174</v>
       </c>
       <c r="B94" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="C94" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D94" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E94">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F94" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>44177</v>
+        <v>44176</v>
       </c>
       <c r="B95" t="s">
-        <v>251</v>
+        <v>43</v>
       </c>
       <c r="C95" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D95" t="s">
-        <v>244</v>
+        <v>18</v>
       </c>
       <c r="E95">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>252</v>
+        <v>44</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>44179</v>
+        <v>44177</v>
       </c>
       <c r="B96" t="s">
-        <v>146</v>
+        <v>251</v>
       </c>
       <c r="C96" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D96" t="s">
-        <v>47</v>
+        <v>244</v>
       </c>
       <c r="E96">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F96" t="s">
-        <v>147</v>
+        <v>252</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>44183</v>
+        <v>44179</v>
       </c>
       <c r="B97" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="C97" t="s">
         <v>234</v>
       </c>
       <c r="D97" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E97">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F97" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>44186</v>
+        <v>44183</v>
       </c>
       <c r="B98" t="s">
-        <v>296</v>
+        <v>45</v>
       </c>
       <c r="C98" t="s">
         <v>234</v>
       </c>
       <c r="D98" t="s">
-        <v>274</v>
+        <v>18</v>
       </c>
       <c r="E98">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F98" t="s">
-        <v>297</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>44208</v>
+        <v>44186</v>
       </c>
       <c r="B99" t="s">
-        <v>148</v>
+        <v>296</v>
       </c>
       <c r="C99" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D99" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E99">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F99" t="s">
-        <v>149</v>
+        <v>297</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>44221</v>
+        <v>44208</v>
       </c>
       <c r="B100" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C100" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D100" t="s">
         <v>47</v>
       </c>
       <c r="E100">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F100" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>44232</v>
+        <v>44221</v>
       </c>
       <c r="B101" t="s">
-        <v>312</v>
+        <v>150</v>
       </c>
       <c r="C101" t="s">
         <v>232</v>
       </c>
       <c r="D101" t="s">
-        <v>302</v>
+        <v>47</v>
       </c>
       <c r="E101">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F101" t="s">
-        <v>313</v>
+        <v>151</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>44239</v>
+        <v>44232</v>
       </c>
       <c r="B102" t="s">
-        <v>153</v>
+        <v>312</v>
       </c>
       <c r="C102" t="s">
         <v>232</v>
       </c>
       <c r="D102" t="s">
-        <v>47</v>
+        <v>302</v>
       </c>
       <c r="E102">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F102" t="s">
-        <v>152</v>
+        <v>313</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>44251</v>
+        <v>44239</v>
       </c>
       <c r="B103" t="s">
-        <v>253</v>
+        <v>153</v>
       </c>
       <c r="C103" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D103" t="s">
-        <v>244</v>
+        <v>47</v>
       </c>
       <c r="E103">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F103" t="s">
-        <v>254</v>
+        <v>152</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>44254</v>
+        <v>44251</v>
       </c>
       <c r="B104" t="s">
-        <v>298</v>
+        <v>253</v>
       </c>
       <c r="C104" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D104" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="E104">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F104" t="s">
-        <v>299</v>
+        <v>254</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>44269</v>
+        <v>44254</v>
       </c>
       <c r="B105" t="s">
-        <v>154</v>
+        <v>298</v>
       </c>
       <c r="C105" t="s">
         <v>234</v>
       </c>
       <c r="D105" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
       <c r="E105">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F105" t="s">
-        <v>155</v>
+        <v>299</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>44263</v>
+        <v>44269</v>
       </c>
       <c r="B106" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C106" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D106" t="s">
         <v>47</v>
       </c>
       <c r="E106">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F106" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>44287</v>
+        <v>44263</v>
       </c>
       <c r="B107" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C107" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D107" t="s">
         <v>47</v>
       </c>
       <c r="E107">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F107" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>44301</v>
+        <v>44287</v>
       </c>
       <c r="B108" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C108" t="s">
         <v>234</v>
@@ -3521,7 +3533,7 @@
         <v>47</v>
       </c>
       <c r="E108">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F108" t="s">
         <v>159</v>
@@ -3529,10 +3541,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>44286</v>
+        <v>44301</v>
       </c>
       <c r="B109" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C109" t="s">
         <v>234</v>
@@ -3541,18 +3553,18 @@
         <v>47</v>
       </c>
       <c r="E109">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F109" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>44299</v>
+        <v>44286</v>
       </c>
       <c r="B110" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C110" t="s">
         <v>234</v>
@@ -3561,18 +3573,18 @@
         <v>47</v>
       </c>
       <c r="E110">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F110" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>44304</v>
+        <v>44299</v>
       </c>
       <c r="B111" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C111" t="s">
         <v>234</v>
@@ -3581,18 +3593,18 @@
         <v>47</v>
       </c>
       <c r="E111">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F111" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>44308</v>
+        <v>44304</v>
       </c>
       <c r="B112" t="s">
-        <v>240</v>
+        <v>165</v>
       </c>
       <c r="C112" t="s">
         <v>234</v>
@@ -3601,181 +3613,181 @@
         <v>47</v>
       </c>
       <c r="E112">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F112" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>44316</v>
+        <v>44308</v>
       </c>
       <c r="B113" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="C113" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D113" t="s">
-        <v>244</v>
+        <v>47</v>
       </c>
       <c r="E113">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F113" t="s">
-        <v>256</v>
+        <v>167</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>44343</v>
+        <v>44316</v>
       </c>
       <c r="B114" t="s">
-        <v>314</v>
+        <v>255</v>
       </c>
       <c r="C114" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D114" t="s">
-        <v>302</v>
+        <v>244</v>
       </c>
       <c r="E114">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F114" t="s">
-        <v>315</v>
+        <v>256</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>44362</v>
+        <v>44343</v>
       </c>
       <c r="B115" t="s">
-        <v>168</v>
+        <v>314</v>
       </c>
       <c r="C115" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D115" t="s">
-        <v>47</v>
+        <v>302</v>
       </c>
       <c r="E115">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F115" t="s">
-        <v>169</v>
+        <v>315</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>44363</v>
+        <v>44362</v>
       </c>
       <c r="B116" t="s">
-        <v>316</v>
+        <v>168</v>
       </c>
       <c r="C116" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D116" t="s">
-        <v>302</v>
+        <v>47</v>
       </c>
       <c r="E116">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F116" t="s">
-        <v>317</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>44374</v>
+        <v>44363</v>
       </c>
       <c r="B117" t="s">
-        <v>170</v>
+        <v>316</v>
       </c>
       <c r="C117" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D117" t="s">
-        <v>47</v>
+        <v>302</v>
       </c>
       <c r="E117">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F117" t="s">
-        <v>171</v>
+        <v>317</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>44392</v>
+        <v>44374</v>
       </c>
       <c r="B118" t="s">
-        <v>318</v>
+        <v>170</v>
       </c>
       <c r="C118" t="s">
         <v>232</v>
       </c>
       <c r="D118" t="s">
-        <v>302</v>
+        <v>47</v>
       </c>
       <c r="E118">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F118" t="s">
-        <v>319</v>
+        <v>171</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>44400</v>
+        <v>44392</v>
       </c>
       <c r="B119" t="s">
-        <v>172</v>
+        <v>318</v>
       </c>
       <c r="C119" t="s">
         <v>232</v>
       </c>
       <c r="D119" t="s">
-        <v>47</v>
+        <v>302</v>
       </c>
       <c r="E119">
         <v>4</v>
       </c>
       <c r="F119" t="s">
-        <v>173</v>
+        <v>319</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>44403</v>
+        <v>44400</v>
       </c>
       <c r="B120" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C120" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D120" t="s">
         <v>47</v>
       </c>
       <c r="E120">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F120" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>44404</v>
+        <v>44403</v>
       </c>
       <c r="B121" t="s">
-        <v>237</v>
+        <v>174</v>
       </c>
       <c r="C121" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D121" t="s">
         <v>47</v>
@@ -3784,75 +3796,75 @@
         <v>6</v>
       </c>
       <c r="F121" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>44406</v>
+        <v>44404</v>
       </c>
       <c r="B122" t="s">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="C122" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D122" t="s">
         <v>47</v>
       </c>
       <c r="E122">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F122" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>44407</v>
+        <v>44406</v>
       </c>
       <c r="B123" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C123" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D123" t="s">
         <v>47</v>
       </c>
       <c r="E123">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F123" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>44419</v>
+        <v>44407</v>
       </c>
       <c r="B124" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C124" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D124" t="s">
         <v>47</v>
       </c>
       <c r="E124">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F124" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>44459</v>
+        <v>44419</v>
       </c>
       <c r="B125" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C125" t="s">
         <v>234</v>
@@ -3861,18 +3873,18 @@
         <v>47</v>
       </c>
       <c r="E125">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F125" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>44468</v>
+        <v>44459</v>
       </c>
       <c r="B126" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C126" t="s">
         <v>234</v>
@@ -3881,121 +3893,121 @@
         <v>47</v>
       </c>
       <c r="E126">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F126" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>44498</v>
+        <v>44468</v>
       </c>
       <c r="B127" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C127" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D127" t="s">
         <v>47</v>
       </c>
       <c r="E127">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F127" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>44503</v>
+        <v>44498</v>
       </c>
       <c r="B128" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C128" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D128" t="s">
         <v>47</v>
       </c>
       <c r="E128">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F128" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>44505</v>
+        <v>44503</v>
       </c>
       <c r="B129" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C129" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D129" t="s">
         <v>47</v>
       </c>
       <c r="E129">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F129" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>44526</v>
+        <v>44505</v>
       </c>
       <c r="B130" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C130" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="D130" t="s">
         <v>47</v>
       </c>
       <c r="E130">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F130" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>44530</v>
+        <v>44526</v>
       </c>
       <c r="B131" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C131" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D131" t="s">
         <v>47</v>
       </c>
       <c r="E131">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F131" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>44545</v>
+        <v>44530</v>
       </c>
       <c r="B132" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C132" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="D132" t="s">
         <v>47</v>
@@ -4004,15 +4016,15 @@
         <v>6</v>
       </c>
       <c r="F132" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>44557</v>
+        <v>44545</v>
       </c>
       <c r="B133" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C133" t="s">
         <v>232</v>
@@ -4021,18 +4033,18 @@
         <v>47</v>
       </c>
       <c r="E133">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F133" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>44565</v>
+        <v>44557</v>
       </c>
       <c r="B134" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C134" t="s">
         <v>232</v>
@@ -4041,18 +4053,18 @@
         <v>47</v>
       </c>
       <c r="E134">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F134" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>44575</v>
+        <v>44565</v>
       </c>
       <c r="B135" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C135" t="s">
         <v>232</v>
@@ -4061,121 +4073,121 @@
         <v>47</v>
       </c>
       <c r="E135">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F135" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>44579</v>
+        <v>44575</v>
       </c>
       <c r="B136" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C136" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D136" t="s">
         <v>47</v>
       </c>
       <c r="E136">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F136" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>44607</v>
+        <v>44579</v>
       </c>
       <c r="B137" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C137" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D137" t="s">
         <v>47</v>
       </c>
       <c r="E137">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F137" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>44609</v>
+        <v>44607</v>
       </c>
       <c r="B138" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C138" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D138" t="s">
         <v>47</v>
       </c>
       <c r="E138">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F138" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>44621</v>
+        <v>44609</v>
       </c>
       <c r="B139" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C139" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D139" t="s">
         <v>47</v>
       </c>
       <c r="E139">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F139" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>44652</v>
+        <v>44621</v>
       </c>
       <c r="B140" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C140" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D140" t="s">
         <v>47</v>
       </c>
       <c r="E140">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F140" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>44669</v>
+        <v>44652</v>
       </c>
       <c r="B141" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C141" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D141" t="s">
         <v>47</v>
@@ -4184,38 +4196,38 @@
         <v>4</v>
       </c>
       <c r="F141" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>44693</v>
+        <v>44669</v>
       </c>
       <c r="B142" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C142" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D142" t="s">
         <v>47</v>
       </c>
       <c r="E142">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F142" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>44733</v>
+        <v>44693</v>
       </c>
       <c r="B143" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C143" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D143" t="s">
         <v>47</v>
@@ -4224,35 +4236,35 @@
         <v>7</v>
       </c>
       <c r="F143" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>44985</v>
+        <v>44733</v>
       </c>
       <c r="B144" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="C144" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D144" t="s">
         <v>47</v>
       </c>
       <c r="E144">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F144" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>45051</v>
+        <v>44985</v>
       </c>
       <c r="B145" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="C145" t="s">
         <v>231</v>
@@ -4261,18 +4273,18 @@
         <v>47</v>
       </c>
       <c r="E145">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F145" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>45057</v>
+        <v>45051</v>
       </c>
       <c r="B146" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C146" t="s">
         <v>231</v>
@@ -4284,6 +4296,26 @@
         <v>8</v>
       </c>
       <c r="F146" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>45057</v>
+      </c>
+      <c r="B147" t="s">
+        <v>224</v>
+      </c>
+      <c r="C147" t="s">
+        <v>231</v>
+      </c>
+      <c r="D147" t="s">
+        <v>47</v>
+      </c>
+      <c r="E147">
+        <v>8</v>
+      </c>
+      <c r="F147" t="s">
         <v>225</v>
       </c>
     </row>
@@ -4296,10 +4328,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0E4DC4-ABC2-455B-9DCE-7C09A6B70159}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4384,6 +4416,14 @@
         <v>303</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>320</v>
+      </c>
+      <c r="B11" t="s">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix Metric Data, Allow Custom Data Upload
</commit_message>
<xml_diff>
--- a/COVID Timeline.xlsx
+++ b/COVID Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BErly\Documents\CA_COVID_TImeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB0006-4808-4228-A100-E9D3B5D466BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50CB6F8-BFDB-431A-975C-12D3D66E3178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{7C800D0D-CC76-4362-974B-133D23204248}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7C800D0D-CC76-4362-974B-133D23204248}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -729,27 +729,9 @@
     <t>The San Francisco Department of Public Health reported two community spread cases within the city. The two cases were unrelated and hospitalized at different hospitals in San Francisco.[39] Yolo County reported its first case, through community transmission.</t>
   </si>
   <si>
-    <t>epi</t>
-  </si>
-  <si>
-    <t>declarations</t>
-  </si>
-  <si>
-    <t>npi</t>
-  </si>
-  <si>
     <t>First confirmed COVID death outside of China</t>
   </si>
   <si>
-    <t>vax</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>treat</t>
-  </si>
-  <si>
     <t xml:space="preserve">CDC and CA recommend return to universal mask wearing. </t>
   </si>
   <si>
@@ -1009,6 +991,24 @@
   </si>
   <si>
     <t>Governor Gavin Newsom announced a call to action to slow the spread of COVID-19 in these hard-hit communities. On Tuesday, July 28, 2020, the California Governor’s Office of Emergency Services (Cal OES) and the California Health and Human Services Agency (CHHS) responded by establishing the Central Valley Task Force.</t>
+  </si>
+  <si>
+    <t>Epidemiologic Milestone</t>
+  </si>
+  <si>
+    <t>Nonpharmaceutical Intervention</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Medications</t>
+  </si>
+  <si>
+    <t>Declarations and Announcementss</t>
+  </si>
+  <si>
+    <t>Vaccination</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6D9AC5-03B3-472C-8251-12875DE34123}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="G148" sqref="G148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1393,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1407,7 +1407,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -1424,19 +1424,19 @@
         <v>43831</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1444,10 +1444,10 @@
         <v>43835</v>
       </c>
       <c r="B4" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1467,7 +1467,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -1487,7 +1487,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -1507,7 +1507,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -1527,7 +1527,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -1547,7 +1547,7 @@
         <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -1564,19 +1564,19 @@
         <v>43858</v>
       </c>
       <c r="B10" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C10" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D10" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1587,7 +1587,7 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1607,7 +1607,7 @@
         <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D12" t="s">
         <v>47</v>
@@ -1627,7 +1627,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D13" t="s">
         <v>47</v>
@@ -1647,7 +1647,7 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D14" t="s">
         <v>47</v>
@@ -1667,7 +1667,7 @@
         <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1687,7 +1687,7 @@
         <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D16" t="s">
         <v>47</v>
@@ -1704,10 +1704,10 @@
         <v>43881</v>
       </c>
       <c r="B17" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C17" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
@@ -1727,7 +1727,7 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
@@ -1747,7 +1747,7 @@
         <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
@@ -1764,19 +1764,19 @@
         <v>43888</v>
       </c>
       <c r="B20" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C20" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D20" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E20">
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1787,7 +1787,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -1804,19 +1804,19 @@
         <v>43890</v>
       </c>
       <c r="B22" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C22" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D22" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E22">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,19 +1824,19 @@
         <v>43892</v>
       </c>
       <c r="B23" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C23" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D23" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E23">
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1847,7 +1847,7 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D24" t="s">
         <v>47</v>
@@ -1867,7 +1867,7 @@
         <v>228</v>
       </c>
       <c r="C25" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D25" t="s">
         <v>226</v>
@@ -1884,19 +1884,19 @@
         <v>43896</v>
       </c>
       <c r="B26" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C26" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D26" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1904,19 +1904,19 @@
         <v>43899</v>
       </c>
       <c r="B27" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C27" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D27" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E27">
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1924,19 +1924,19 @@
         <v>43899</v>
       </c>
       <c r="B28" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C28" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D28" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>
@@ -1967,7 +1967,7 @@
         <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D30" t="s">
         <v>47</v>
@@ -1987,7 +1987,7 @@
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -2007,7 +2007,7 @@
         <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D32" t="s">
         <v>47</v>
@@ -2027,7 +2027,7 @@
         <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D33" t="s">
         <v>47</v>
@@ -2047,7 +2047,7 @@
         <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D34" t="s">
         <v>65</v>
@@ -2064,19 +2064,19 @@
         <v>43903</v>
       </c>
       <c r="B35" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C35" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D35" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E35">
         <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D36" t="s">
         <v>18</v>
@@ -2104,10 +2104,10 @@
         <v>43905</v>
       </c>
       <c r="B37" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C37" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D37" t="s">
         <v>47</v>
@@ -2127,7 +2127,7 @@
         <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D38" t="s">
         <v>47</v>
@@ -2147,7 +2147,7 @@
         <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
@@ -2167,7 +2167,7 @@
         <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D40" t="s">
         <v>47</v>
@@ -2187,7 +2187,7 @@
         <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D41" t="s">
         <v>47</v>
@@ -2204,19 +2204,19 @@
         <v>43908</v>
       </c>
       <c r="B42" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C42" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D42" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E42">
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
         <v>84</v>
       </c>
       <c r="C43" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D43" t="s">
         <v>47</v>
@@ -2247,7 +2247,7 @@
         <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D44" t="s">
         <v>47</v>
@@ -2264,19 +2264,19 @@
         <v>43910</v>
       </c>
       <c r="B45" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C45" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D45" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E45">
         <v>4</v>
       </c>
       <c r="F45" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2284,19 +2284,19 @@
         <v>43910</v>
       </c>
       <c r="B46" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C46" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D46" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E46">
         <v>6</v>
       </c>
       <c r="F46" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
@@ -2327,7 +2327,7 @@
         <v>88</v>
       </c>
       <c r="C48" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D48" t="s">
         <v>47</v>
@@ -2344,19 +2344,19 @@
         <v>43922</v>
       </c>
       <c r="B49" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C49" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D49" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E49">
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2364,19 +2364,19 @@
         <v>43923</v>
       </c>
       <c r="B50" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C50" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D50" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E50">
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2387,7 +2387,7 @@
         <v>90</v>
       </c>
       <c r="C51" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
@@ -2407,7 +2407,7 @@
         <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D52" t="s">
         <v>47</v>
@@ -2427,7 +2427,7 @@
         <v>94</v>
       </c>
       <c r="C53" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D53" t="s">
         <v>47</v>
@@ -2444,19 +2444,19 @@
         <v>43934</v>
       </c>
       <c r="B54" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C54" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D54" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E54">
         <v>4</v>
       </c>
       <c r="F54" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2467,7 +2467,7 @@
         <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -2487,7 +2487,7 @@
         <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D56" t="s">
         <v>47</v>
@@ -2507,7 +2507,7 @@
         <v>98</v>
       </c>
       <c r="C57" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D57" t="s">
         <v>47</v>
@@ -2524,19 +2524,19 @@
         <v>43944</v>
       </c>
       <c r="B58" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C58" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D58" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E58">
         <v>3</v>
       </c>
       <c r="F58" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,10 +2544,10 @@
         <v>43949</v>
       </c>
       <c r="B59" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C59" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D59" t="s">
         <v>47</v>
@@ -2567,7 +2567,7 @@
         <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
@@ -2587,7 +2587,7 @@
         <v>101</v>
       </c>
       <c r="C61" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D61" t="s">
         <v>47</v>
@@ -2607,7 +2607,7 @@
         <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D62" t="s">
         <v>47</v>
@@ -2627,7 +2627,7 @@
         <v>105</v>
       </c>
       <c r="C63" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D63" t="s">
         <v>47</v>
@@ -2647,7 +2647,7 @@
         <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D64" t="s">
         <v>47</v>
@@ -2667,7 +2667,7 @@
         <v>109</v>
       </c>
       <c r="C65" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D65" t="s">
         <v>47</v>
@@ -2684,19 +2684,19 @@
         <v>43991</v>
       </c>
       <c r="B66" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C66" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D66" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E66">
         <v>4</v>
       </c>
       <c r="F66" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2707,7 +2707,7 @@
         <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D67" t="s">
         <v>47</v>
@@ -2727,7 +2727,7 @@
         <v>113</v>
       </c>
       <c r="C68" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D68" t="s">
         <v>47</v>
@@ -2747,7 +2747,7 @@
         <v>122</v>
       </c>
       <c r="C69" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D69" t="s">
         <v>47</v>
@@ -2767,7 +2767,7 @@
         <v>116</v>
       </c>
       <c r="C70" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D70" t="s">
         <v>47</v>
@@ -2787,7 +2787,7 @@
         <v>118</v>
       </c>
       <c r="C71" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D71" t="s">
         <v>47</v>
@@ -2807,7 +2807,7 @@
         <v>120</v>
       </c>
       <c r="C72" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D72" t="s">
         <v>47</v>
@@ -2827,7 +2827,7 @@
         <v>123</v>
       </c>
       <c r="C73" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D73" t="s">
         <v>47</v>
@@ -2847,7 +2847,7 @@
         <v>125</v>
       </c>
       <c r="C74" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D74" t="s">
         <v>47</v>
@@ -2864,19 +2864,19 @@
         <v>44040</v>
       </c>
       <c r="B75" t="s">
+        <v>316</v>
+      </c>
+      <c r="C75" t="s">
         <v>322</v>
       </c>
-      <c r="C75" t="s">
-        <v>231</v>
-      </c>
       <c r="D75" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E75">
         <v>6</v>
       </c>
       <c r="F75" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2884,19 +2884,19 @@
         <v>44046</v>
       </c>
       <c r="B76" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C76" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D76" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E76">
         <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2904,19 +2904,19 @@
         <v>44054</v>
       </c>
       <c r="B77" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C77" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D77" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E77">
         <v>4</v>
       </c>
       <c r="F77" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2927,7 +2927,7 @@
         <v>127</v>
       </c>
       <c r="C78" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D78" t="s">
         <v>47</v>
@@ -2944,10 +2944,10 @@
         <v>44071</v>
       </c>
       <c r="B79" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C79" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D79" t="s">
         <v>47</v>
@@ -2967,7 +2967,7 @@
         <v>130</v>
       </c>
       <c r="C80" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D80" t="s">
         <v>47</v>
@@ -2987,7 +2987,7 @@
         <v>39</v>
       </c>
       <c r="C81" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D81" t="s">
         <v>18</v>
@@ -3004,19 +3004,19 @@
         <v>44106</v>
       </c>
       <c r="B82" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C82" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D82" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E82">
         <v>6</v>
       </c>
       <c r="F82" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3024,19 +3024,19 @@
         <v>44117</v>
       </c>
       <c r="B83" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C83" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D83" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E83">
         <v>6</v>
       </c>
       <c r="F83" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -3044,19 +3044,19 @@
         <v>44126</v>
       </c>
       <c r="B84" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C84" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D84" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E84">
         <v>5</v>
       </c>
       <c r="F84" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -3064,19 +3064,19 @@
         <v>44132</v>
       </c>
       <c r="B85" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C85" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D85" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E85">
         <v>5</v>
       </c>
       <c r="F85" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3087,7 +3087,7 @@
         <v>132</v>
       </c>
       <c r="C86" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D86" t="s">
         <v>47</v>
@@ -3104,19 +3104,19 @@
         <v>44147</v>
       </c>
       <c r="B87" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C87" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D87" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E87">
         <v>7</v>
       </c>
       <c r="F87" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3127,7 +3127,7 @@
         <v>134</v>
       </c>
       <c r="C88" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D88" t="s">
         <v>47</v>
@@ -3147,7 +3147,7 @@
         <v>136</v>
       </c>
       <c r="C89" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D89" t="s">
         <v>47</v>
@@ -3167,7 +3167,7 @@
         <v>138</v>
       </c>
       <c r="C90" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D90" t="s">
         <v>47</v>
@@ -3187,7 +3187,7 @@
         <v>41</v>
       </c>
       <c r="C91" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D91" t="s">
         <v>18</v>
@@ -3207,7 +3207,7 @@
         <v>140</v>
       </c>
       <c r="C92" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D92" t="s">
         <v>47</v>
@@ -3227,7 +3227,7 @@
         <v>143</v>
       </c>
       <c r="C93" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D93" t="s">
         <v>47</v>
@@ -3247,7 +3247,7 @@
         <v>144</v>
       </c>
       <c r="C94" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D94" t="s">
         <v>47</v>
@@ -3267,7 +3267,7 @@
         <v>43</v>
       </c>
       <c r="C95" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D95" t="s">
         <v>18</v>
@@ -3284,19 +3284,19 @@
         <v>44177</v>
       </c>
       <c r="B96" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C96" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D96" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E96">
         <v>6</v>
       </c>
       <c r="F96" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3307,7 +3307,7 @@
         <v>146</v>
       </c>
       <c r="C97" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D97" t="s">
         <v>47</v>
@@ -3327,7 +3327,7 @@
         <v>45</v>
       </c>
       <c r="C98" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D98" t="s">
         <v>18</v>
@@ -3344,19 +3344,19 @@
         <v>44186</v>
       </c>
       <c r="B99" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C99" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D99" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E99">
         <v>7</v>
       </c>
       <c r="F99" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3367,7 +3367,7 @@
         <v>148</v>
       </c>
       <c r="C100" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D100" t="s">
         <v>47</v>
@@ -3387,7 +3387,7 @@
         <v>150</v>
       </c>
       <c r="C101" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D101" t="s">
         <v>47</v>
@@ -3404,19 +3404,19 @@
         <v>44232</v>
       </c>
       <c r="B102" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C102" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D102" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E102">
         <v>6</v>
       </c>
       <c r="F102" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3427,7 +3427,7 @@
         <v>153</v>
       </c>
       <c r="C103" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D103" t="s">
         <v>47</v>
@@ -3444,19 +3444,19 @@
         <v>44251</v>
       </c>
       <c r="B104" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C104" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D104" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E104">
         <v>5</v>
       </c>
       <c r="F104" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3464,19 +3464,19 @@
         <v>44254</v>
       </c>
       <c r="B105" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C105" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D105" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E105">
         <v>6</v>
       </c>
       <c r="F105" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3487,7 +3487,7 @@
         <v>154</v>
       </c>
       <c r="C106" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D106" t="s">
         <v>47</v>
@@ -3507,7 +3507,7 @@
         <v>156</v>
       </c>
       <c r="C107" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D107" t="s">
         <v>47</v>
@@ -3527,7 +3527,7 @@
         <v>158</v>
       </c>
       <c r="C108" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D108" t="s">
         <v>47</v>
@@ -3547,7 +3547,7 @@
         <v>160</v>
       </c>
       <c r="C109" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D109" t="s">
         <v>47</v>
@@ -3567,7 +3567,7 @@
         <v>161</v>
       </c>
       <c r="C110" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D110" t="s">
         <v>47</v>
@@ -3587,7 +3587,7 @@
         <v>163</v>
       </c>
       <c r="C111" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D111" t="s">
         <v>47</v>
@@ -3607,7 +3607,7 @@
         <v>165</v>
       </c>
       <c r="C112" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D112" t="s">
         <v>47</v>
@@ -3624,10 +3624,10 @@
         <v>44308</v>
       </c>
       <c r="B113" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C113" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D113" t="s">
         <v>47</v>
@@ -3644,19 +3644,19 @@
         <v>44316</v>
       </c>
       <c r="B114" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C114" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D114" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E114">
         <v>4</v>
       </c>
       <c r="F114" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3664,19 +3664,19 @@
         <v>44343</v>
       </c>
       <c r="B115" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C115" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D115" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E115">
         <v>5</v>
       </c>
       <c r="F115" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3687,7 +3687,7 @@
         <v>168</v>
       </c>
       <c r="C116" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D116" t="s">
         <v>47</v>
@@ -3704,19 +3704,19 @@
         <v>44363</v>
       </c>
       <c r="B117" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C117" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D117" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E117">
         <v>3</v>
       </c>
       <c r="F117" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3727,7 +3727,7 @@
         <v>170</v>
       </c>
       <c r="C118" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D118" t="s">
         <v>47</v>
@@ -3744,19 +3744,19 @@
         <v>44392</v>
       </c>
       <c r="B119" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C119" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D119" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E119">
         <v>4</v>
       </c>
       <c r="F119" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3767,7 +3767,7 @@
         <v>172</v>
       </c>
       <c r="C120" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D120" t="s">
         <v>47</v>
@@ -3787,7 +3787,7 @@
         <v>174</v>
       </c>
       <c r="C121" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D121" t="s">
         <v>47</v>
@@ -3804,10 +3804,10 @@
         <v>44404</v>
       </c>
       <c r="B122" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C122" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D122" t="s">
         <v>47</v>
@@ -3827,7 +3827,7 @@
         <v>177</v>
       </c>
       <c r="C123" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D123" t="s">
         <v>47</v>
@@ -3847,7 +3847,7 @@
         <v>179</v>
       </c>
       <c r="C124" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D124" t="s">
         <v>47</v>
@@ -3867,7 +3867,7 @@
         <v>181</v>
       </c>
       <c r="C125" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D125" t="s">
         <v>47</v>
@@ -3887,7 +3887,7 @@
         <v>183</v>
       </c>
       <c r="C126" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D126" t="s">
         <v>47</v>
@@ -3907,7 +3907,7 @@
         <v>185</v>
       </c>
       <c r="C127" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D127" t="s">
         <v>47</v>
@@ -3927,7 +3927,7 @@
         <v>187</v>
       </c>
       <c r="C128" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D128" t="s">
         <v>47</v>
@@ -3947,7 +3947,7 @@
         <v>189</v>
       </c>
       <c r="C129" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D129" t="s">
         <v>47</v>
@@ -3967,7 +3967,7 @@
         <v>191</v>
       </c>
       <c r="C130" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D130" t="s">
         <v>47</v>
@@ -3987,7 +3987,7 @@
         <v>193</v>
       </c>
       <c r="C131" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D131" t="s">
         <v>47</v>
@@ -4007,7 +4007,7 @@
         <v>195</v>
       </c>
       <c r="C132" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D132" t="s">
         <v>47</v>
@@ -4027,7 +4027,7 @@
         <v>197</v>
       </c>
       <c r="C133" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D133" t="s">
         <v>47</v>
@@ -4047,7 +4047,7 @@
         <v>199</v>
       </c>
       <c r="C134" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D134" t="s">
         <v>47</v>
@@ -4067,7 +4067,7 @@
         <v>201</v>
       </c>
       <c r="C135" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D135" t="s">
         <v>47</v>
@@ -4087,7 +4087,7 @@
         <v>203</v>
       </c>
       <c r="C136" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D136" t="s">
         <v>47</v>
@@ -4107,7 +4107,7 @@
         <v>205</v>
       </c>
       <c r="C137" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D137" t="s">
         <v>47</v>
@@ -4127,7 +4127,7 @@
         <v>211</v>
       </c>
       <c r="C138" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D138" t="s">
         <v>47</v>
@@ -4147,7 +4147,7 @@
         <v>209</v>
       </c>
       <c r="C139" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D139" t="s">
         <v>47</v>
@@ -4167,7 +4167,7 @@
         <v>207</v>
       </c>
       <c r="C140" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D140" t="s">
         <v>47</v>
@@ -4187,7 +4187,7 @@
         <v>213</v>
       </c>
       <c r="C141" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D141" t="s">
         <v>47</v>
@@ -4207,7 +4207,7 @@
         <v>215</v>
       </c>
       <c r="C142" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D142" t="s">
         <v>47</v>
@@ -4227,7 +4227,7 @@
         <v>218</v>
       </c>
       <c r="C143" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D143" t="s">
         <v>47</v>
@@ -4247,7 +4247,7 @@
         <v>219</v>
       </c>
       <c r="C144" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D144" t="s">
         <v>47</v>
@@ -4264,10 +4264,10 @@
         <v>44985</v>
       </c>
       <c r="B145" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C145" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D145" t="s">
         <v>47</v>
@@ -4287,7 +4287,7 @@
         <v>222</v>
       </c>
       <c r="C146" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D146" t="s">
         <v>47</v>
@@ -4307,7 +4307,7 @@
         <v>224</v>
       </c>
       <c r="C147" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D147" t="s">
         <v>47</v>
@@ -4330,8 +4330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0E4DC4-ABC2-455B-9DCE-7C09A6B70159}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4386,42 +4386,42 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B8" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B9" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Timeline with Blueprint Data
</commit_message>
<xml_diff>
--- a/COVID Timeline.xlsx
+++ b/COVID Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BErly\Documents\CA_COVID_TImeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB0006-4808-4228-A100-E9D3B5D466BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50CB6F8-BFDB-431A-975C-12D3D66E3178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{7C800D0D-CC76-4362-974B-133D23204248}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7C800D0D-CC76-4362-974B-133D23204248}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -729,27 +729,9 @@
     <t>The San Francisco Department of Public Health reported two community spread cases within the city. The two cases were unrelated and hospitalized at different hospitals in San Francisco.[39] Yolo County reported its first case, through community transmission.</t>
   </si>
   <si>
-    <t>epi</t>
-  </si>
-  <si>
-    <t>declarations</t>
-  </si>
-  <si>
-    <t>npi</t>
-  </si>
-  <si>
     <t>First confirmed COVID death outside of China</t>
   </si>
   <si>
-    <t>vax</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>treat</t>
-  </si>
-  <si>
     <t xml:space="preserve">CDC and CA recommend return to universal mask wearing. </t>
   </si>
   <si>
@@ -1009,6 +991,24 @@
   </si>
   <si>
     <t>Governor Gavin Newsom announced a call to action to slow the spread of COVID-19 in these hard-hit communities. On Tuesday, July 28, 2020, the California Governor’s Office of Emergency Services (Cal OES) and the California Health and Human Services Agency (CHHS) responded by establishing the Central Valley Task Force.</t>
+  </si>
+  <si>
+    <t>Epidemiologic Milestone</t>
+  </si>
+  <si>
+    <t>Nonpharmaceutical Intervention</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Medications</t>
+  </si>
+  <si>
+    <t>Declarations and Announcementss</t>
+  </si>
+  <si>
+    <t>Vaccination</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6D9AC5-03B3-472C-8251-12875DE34123}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="G148" sqref="G148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1393,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -1407,7 +1407,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -1424,19 +1424,19 @@
         <v>43831</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1444,10 +1444,10 @@
         <v>43835</v>
       </c>
       <c r="B4" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1467,7 +1467,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -1487,7 +1487,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -1507,7 +1507,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -1527,7 +1527,7 @@
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -1547,7 +1547,7 @@
         <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -1564,19 +1564,19 @@
         <v>43858</v>
       </c>
       <c r="B10" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C10" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D10" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1587,7 +1587,7 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1607,7 +1607,7 @@
         <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D12" t="s">
         <v>47</v>
@@ -1627,7 +1627,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D13" t="s">
         <v>47</v>
@@ -1647,7 +1647,7 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D14" t="s">
         <v>47</v>
@@ -1667,7 +1667,7 @@
         <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1687,7 +1687,7 @@
         <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D16" t="s">
         <v>47</v>
@@ -1704,10 +1704,10 @@
         <v>43881</v>
       </c>
       <c r="B17" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C17" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
@@ -1727,7 +1727,7 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
@@ -1747,7 +1747,7 @@
         <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D19" t="s">
         <v>47</v>
@@ -1764,19 +1764,19 @@
         <v>43888</v>
       </c>
       <c r="B20" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C20" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D20" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E20">
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1787,7 +1787,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -1804,19 +1804,19 @@
         <v>43890</v>
       </c>
       <c r="B22" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C22" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D22" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E22">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,19 +1824,19 @@
         <v>43892</v>
       </c>
       <c r="B23" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C23" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D23" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E23">
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1847,7 +1847,7 @@
         <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D24" t="s">
         <v>47</v>
@@ -1867,7 +1867,7 @@
         <v>228</v>
       </c>
       <c r="C25" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D25" t="s">
         <v>226</v>
@@ -1884,19 +1884,19 @@
         <v>43896</v>
       </c>
       <c r="B26" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C26" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D26" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1904,19 +1904,19 @@
         <v>43899</v>
       </c>
       <c r="B27" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C27" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D27" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E27">
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1924,19 +1924,19 @@
         <v>43899</v>
       </c>
       <c r="B28" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C28" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D28" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E28">
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>
@@ -1967,7 +1967,7 @@
         <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D30" t="s">
         <v>47</v>
@@ -1987,7 +1987,7 @@
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -2007,7 +2007,7 @@
         <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D32" t="s">
         <v>47</v>
@@ -2027,7 +2027,7 @@
         <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D33" t="s">
         <v>47</v>
@@ -2047,7 +2047,7 @@
         <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D34" t="s">
         <v>65</v>
@@ -2064,19 +2064,19 @@
         <v>43903</v>
       </c>
       <c r="B35" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C35" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D35" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E35">
         <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D36" t="s">
         <v>18</v>
@@ -2104,10 +2104,10 @@
         <v>43905</v>
       </c>
       <c r="B37" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C37" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D37" t="s">
         <v>47</v>
@@ -2127,7 +2127,7 @@
         <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D38" t="s">
         <v>47</v>
@@ -2147,7 +2147,7 @@
         <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
@@ -2167,7 +2167,7 @@
         <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D40" t="s">
         <v>47</v>
@@ -2187,7 +2187,7 @@
         <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D41" t="s">
         <v>47</v>
@@ -2204,19 +2204,19 @@
         <v>43908</v>
       </c>
       <c r="B42" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C42" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D42" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E42">
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
         <v>84</v>
       </c>
       <c r="C43" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D43" t="s">
         <v>47</v>
@@ -2247,7 +2247,7 @@
         <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D44" t="s">
         <v>47</v>
@@ -2264,19 +2264,19 @@
         <v>43910</v>
       </c>
       <c r="B45" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C45" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D45" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E45">
         <v>4</v>
       </c>
       <c r="F45" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -2284,19 +2284,19 @@
         <v>43910</v>
       </c>
       <c r="B46" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C46" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D46" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E46">
         <v>6</v>
       </c>
       <c r="F46" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D47" t="s">
         <v>18</v>
@@ -2327,7 +2327,7 @@
         <v>88</v>
       </c>
       <c r="C48" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D48" t="s">
         <v>47</v>
@@ -2344,19 +2344,19 @@
         <v>43922</v>
       </c>
       <c r="B49" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C49" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D49" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E49">
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2364,19 +2364,19 @@
         <v>43923</v>
       </c>
       <c r="B50" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C50" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D50" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E50">
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2387,7 +2387,7 @@
         <v>90</v>
       </c>
       <c r="C51" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
@@ -2407,7 +2407,7 @@
         <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D52" t="s">
         <v>47</v>
@@ -2427,7 +2427,7 @@
         <v>94</v>
       </c>
       <c r="C53" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D53" t="s">
         <v>47</v>
@@ -2444,19 +2444,19 @@
         <v>43934</v>
       </c>
       <c r="B54" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C54" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D54" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E54">
         <v>4</v>
       </c>
       <c r="F54" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2467,7 +2467,7 @@
         <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -2487,7 +2487,7 @@
         <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D56" t="s">
         <v>47</v>
@@ -2507,7 +2507,7 @@
         <v>98</v>
       </c>
       <c r="C57" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D57" t="s">
         <v>47</v>
@@ -2524,19 +2524,19 @@
         <v>43944</v>
       </c>
       <c r="B58" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C58" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D58" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E58">
         <v>3</v>
       </c>
       <c r="F58" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,10 +2544,10 @@
         <v>43949</v>
       </c>
       <c r="B59" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C59" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D59" t="s">
         <v>47</v>
@@ -2567,7 +2567,7 @@
         <v>37</v>
       </c>
       <c r="C60" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D60" t="s">
         <v>18</v>
@@ -2587,7 +2587,7 @@
         <v>101</v>
       </c>
       <c r="C61" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D61" t="s">
         <v>47</v>
@@ -2607,7 +2607,7 @@
         <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D62" t="s">
         <v>47</v>
@@ -2627,7 +2627,7 @@
         <v>105</v>
       </c>
       <c r="C63" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D63" t="s">
         <v>47</v>
@@ -2647,7 +2647,7 @@
         <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D64" t="s">
         <v>47</v>
@@ -2667,7 +2667,7 @@
         <v>109</v>
       </c>
       <c r="C65" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D65" t="s">
         <v>47</v>
@@ -2684,19 +2684,19 @@
         <v>43991</v>
       </c>
       <c r="B66" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C66" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D66" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E66">
         <v>4</v>
       </c>
       <c r="F66" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2707,7 +2707,7 @@
         <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D67" t="s">
         <v>47</v>
@@ -2727,7 +2727,7 @@
         <v>113</v>
       </c>
       <c r="C68" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D68" t="s">
         <v>47</v>
@@ -2747,7 +2747,7 @@
         <v>122</v>
       </c>
       <c r="C69" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D69" t="s">
         <v>47</v>
@@ -2767,7 +2767,7 @@
         <v>116</v>
       </c>
       <c r="C70" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D70" t="s">
         <v>47</v>
@@ -2787,7 +2787,7 @@
         <v>118</v>
       </c>
       <c r="C71" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D71" t="s">
         <v>47</v>
@@ -2807,7 +2807,7 @@
         <v>120</v>
       </c>
       <c r="C72" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D72" t="s">
         <v>47</v>
@@ -2827,7 +2827,7 @@
         <v>123</v>
       </c>
       <c r="C73" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D73" t="s">
         <v>47</v>
@@ -2847,7 +2847,7 @@
         <v>125</v>
       </c>
       <c r="C74" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D74" t="s">
         <v>47</v>
@@ -2864,19 +2864,19 @@
         <v>44040</v>
       </c>
       <c r="B75" t="s">
+        <v>316</v>
+      </c>
+      <c r="C75" t="s">
         <v>322</v>
       </c>
-      <c r="C75" t="s">
-        <v>231</v>
-      </c>
       <c r="D75" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E75">
         <v>6</v>
       </c>
       <c r="F75" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2884,19 +2884,19 @@
         <v>44046</v>
       </c>
       <c r="B76" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C76" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D76" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E76">
         <v>7</v>
       </c>
       <c r="F76" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2904,19 +2904,19 @@
         <v>44054</v>
       </c>
       <c r="B77" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C77" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D77" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E77">
         <v>4</v>
       </c>
       <c r="F77" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2927,7 +2927,7 @@
         <v>127</v>
       </c>
       <c r="C78" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D78" t="s">
         <v>47</v>
@@ -2944,10 +2944,10 @@
         <v>44071</v>
       </c>
       <c r="B79" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C79" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D79" t="s">
         <v>47</v>
@@ -2967,7 +2967,7 @@
         <v>130</v>
       </c>
       <c r="C80" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D80" t="s">
         <v>47</v>
@@ -2987,7 +2987,7 @@
         <v>39</v>
       </c>
       <c r="C81" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D81" t="s">
         <v>18</v>
@@ -3004,19 +3004,19 @@
         <v>44106</v>
       </c>
       <c r="B82" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C82" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D82" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E82">
         <v>6</v>
       </c>
       <c r="F82" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -3024,19 +3024,19 @@
         <v>44117</v>
       </c>
       <c r="B83" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C83" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D83" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E83">
         <v>6</v>
       </c>
       <c r="F83" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -3044,19 +3044,19 @@
         <v>44126</v>
       </c>
       <c r="B84" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C84" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D84" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E84">
         <v>5</v>
       </c>
       <c r="F84" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -3064,19 +3064,19 @@
         <v>44132</v>
       </c>
       <c r="B85" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C85" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D85" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E85">
         <v>5</v>
       </c>
       <c r="F85" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3087,7 +3087,7 @@
         <v>132</v>
       </c>
       <c r="C86" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D86" t="s">
         <v>47</v>
@@ -3104,19 +3104,19 @@
         <v>44147</v>
       </c>
       <c r="B87" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C87" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D87" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E87">
         <v>7</v>
       </c>
       <c r="F87" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -3127,7 +3127,7 @@
         <v>134</v>
       </c>
       <c r="C88" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D88" t="s">
         <v>47</v>
@@ -3147,7 +3147,7 @@
         <v>136</v>
       </c>
       <c r="C89" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D89" t="s">
         <v>47</v>
@@ -3167,7 +3167,7 @@
         <v>138</v>
       </c>
       <c r="C90" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D90" t="s">
         <v>47</v>
@@ -3187,7 +3187,7 @@
         <v>41</v>
       </c>
       <c r="C91" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D91" t="s">
         <v>18</v>
@@ -3207,7 +3207,7 @@
         <v>140</v>
       </c>
       <c r="C92" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D92" t="s">
         <v>47</v>
@@ -3227,7 +3227,7 @@
         <v>143</v>
       </c>
       <c r="C93" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D93" t="s">
         <v>47</v>
@@ -3247,7 +3247,7 @@
         <v>144</v>
       </c>
       <c r="C94" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D94" t="s">
         <v>47</v>
@@ -3267,7 +3267,7 @@
         <v>43</v>
       </c>
       <c r="C95" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D95" t="s">
         <v>18</v>
@@ -3284,19 +3284,19 @@
         <v>44177</v>
       </c>
       <c r="B96" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C96" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D96" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E96">
         <v>6</v>
       </c>
       <c r="F96" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3307,7 +3307,7 @@
         <v>146</v>
       </c>
       <c r="C97" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D97" t="s">
         <v>47</v>
@@ -3327,7 +3327,7 @@
         <v>45</v>
       </c>
       <c r="C98" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D98" t="s">
         <v>18</v>
@@ -3344,19 +3344,19 @@
         <v>44186</v>
       </c>
       <c r="B99" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C99" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D99" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E99">
         <v>7</v>
       </c>
       <c r="F99" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -3367,7 +3367,7 @@
         <v>148</v>
       </c>
       <c r="C100" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D100" t="s">
         <v>47</v>
@@ -3387,7 +3387,7 @@
         <v>150</v>
       </c>
       <c r="C101" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D101" t="s">
         <v>47</v>
@@ -3404,19 +3404,19 @@
         <v>44232</v>
       </c>
       <c r="B102" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C102" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D102" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E102">
         <v>6</v>
       </c>
       <c r="F102" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -3427,7 +3427,7 @@
         <v>153</v>
       </c>
       <c r="C103" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D103" t="s">
         <v>47</v>
@@ -3444,19 +3444,19 @@
         <v>44251</v>
       </c>
       <c r="B104" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C104" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D104" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E104">
         <v>5</v>
       </c>
       <c r="F104" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -3464,19 +3464,19 @@
         <v>44254</v>
       </c>
       <c r="B105" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C105" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D105" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E105">
         <v>6</v>
       </c>
       <c r="F105" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -3487,7 +3487,7 @@
         <v>154</v>
       </c>
       <c r="C106" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D106" t="s">
         <v>47</v>
@@ -3507,7 +3507,7 @@
         <v>156</v>
       </c>
       <c r="C107" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D107" t="s">
         <v>47</v>
@@ -3527,7 +3527,7 @@
         <v>158</v>
       </c>
       <c r="C108" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D108" t="s">
         <v>47</v>
@@ -3547,7 +3547,7 @@
         <v>160</v>
       </c>
       <c r="C109" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D109" t="s">
         <v>47</v>
@@ -3567,7 +3567,7 @@
         <v>161</v>
       </c>
       <c r="C110" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D110" t="s">
         <v>47</v>
@@ -3587,7 +3587,7 @@
         <v>163</v>
       </c>
       <c r="C111" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D111" t="s">
         <v>47</v>
@@ -3607,7 +3607,7 @@
         <v>165</v>
       </c>
       <c r="C112" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D112" t="s">
         <v>47</v>
@@ -3624,10 +3624,10 @@
         <v>44308</v>
       </c>
       <c r="B113" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C113" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D113" t="s">
         <v>47</v>
@@ -3644,19 +3644,19 @@
         <v>44316</v>
       </c>
       <c r="B114" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C114" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D114" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E114">
         <v>4</v>
       </c>
       <c r="F114" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3664,19 +3664,19 @@
         <v>44343</v>
       </c>
       <c r="B115" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C115" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D115" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E115">
         <v>5</v>
       </c>
       <c r="F115" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3687,7 +3687,7 @@
         <v>168</v>
       </c>
       <c r="C116" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D116" t="s">
         <v>47</v>
@@ -3704,19 +3704,19 @@
         <v>44363</v>
       </c>
       <c r="B117" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C117" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D117" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E117">
         <v>3</v>
       </c>
       <c r="F117" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3727,7 +3727,7 @@
         <v>170</v>
       </c>
       <c r="C118" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D118" t="s">
         <v>47</v>
@@ -3744,19 +3744,19 @@
         <v>44392</v>
       </c>
       <c r="B119" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C119" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D119" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E119">
         <v>4</v>
       </c>
       <c r="F119" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -3767,7 +3767,7 @@
         <v>172</v>
       </c>
       <c r="C120" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D120" t="s">
         <v>47</v>
@@ -3787,7 +3787,7 @@
         <v>174</v>
       </c>
       <c r="C121" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D121" t="s">
         <v>47</v>
@@ -3804,10 +3804,10 @@
         <v>44404</v>
       </c>
       <c r="B122" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C122" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D122" t="s">
         <v>47</v>
@@ -3827,7 +3827,7 @@
         <v>177</v>
       </c>
       <c r="C123" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D123" t="s">
         <v>47</v>
@@ -3847,7 +3847,7 @@
         <v>179</v>
       </c>
       <c r="C124" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D124" t="s">
         <v>47</v>
@@ -3867,7 +3867,7 @@
         <v>181</v>
       </c>
       <c r="C125" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D125" t="s">
         <v>47</v>
@@ -3887,7 +3887,7 @@
         <v>183</v>
       </c>
       <c r="C126" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D126" t="s">
         <v>47</v>
@@ -3907,7 +3907,7 @@
         <v>185</v>
       </c>
       <c r="C127" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D127" t="s">
         <v>47</v>
@@ -3927,7 +3927,7 @@
         <v>187</v>
       </c>
       <c r="C128" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D128" t="s">
         <v>47</v>
@@ -3947,7 +3947,7 @@
         <v>189</v>
       </c>
       <c r="C129" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D129" t="s">
         <v>47</v>
@@ -3967,7 +3967,7 @@
         <v>191</v>
       </c>
       <c r="C130" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D130" t="s">
         <v>47</v>
@@ -3987,7 +3987,7 @@
         <v>193</v>
       </c>
       <c r="C131" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D131" t="s">
         <v>47</v>
@@ -4007,7 +4007,7 @@
         <v>195</v>
       </c>
       <c r="C132" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="D132" t="s">
         <v>47</v>
@@ -4027,7 +4027,7 @@
         <v>197</v>
       </c>
       <c r="C133" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D133" t="s">
         <v>47</v>
@@ -4047,7 +4047,7 @@
         <v>199</v>
       </c>
       <c r="C134" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D134" t="s">
         <v>47</v>
@@ -4067,7 +4067,7 @@
         <v>201</v>
       </c>
       <c r="C135" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D135" t="s">
         <v>47</v>
@@ -4087,7 +4087,7 @@
         <v>203</v>
       </c>
       <c r="C136" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D136" t="s">
         <v>47</v>
@@ -4107,7 +4107,7 @@
         <v>205</v>
       </c>
       <c r="C137" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="D137" t="s">
         <v>47</v>
@@ -4127,7 +4127,7 @@
         <v>211</v>
       </c>
       <c r="C138" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D138" t="s">
         <v>47</v>
@@ -4147,7 +4147,7 @@
         <v>209</v>
       </c>
       <c r="C139" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D139" t="s">
         <v>47</v>
@@ -4167,7 +4167,7 @@
         <v>207</v>
       </c>
       <c r="C140" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D140" t="s">
         <v>47</v>
@@ -4187,7 +4187,7 @@
         <v>213</v>
       </c>
       <c r="C141" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D141" t="s">
         <v>47</v>
@@ -4207,7 +4207,7 @@
         <v>215</v>
       </c>
       <c r="C142" t="s">
-        <v>232</v>
+        <v>319</v>
       </c>
       <c r="D142" t="s">
         <v>47</v>
@@ -4227,7 +4227,7 @@
         <v>218</v>
       </c>
       <c r="C143" t="s">
-        <v>230</v>
+        <v>318</v>
       </c>
       <c r="D143" t="s">
         <v>47</v>
@@ -4247,7 +4247,7 @@
         <v>219</v>
       </c>
       <c r="C144" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="D144" t="s">
         <v>47</v>
@@ -4264,10 +4264,10 @@
         <v>44985</v>
       </c>
       <c r="B145" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C145" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D145" t="s">
         <v>47</v>
@@ -4287,7 +4287,7 @@
         <v>222</v>
       </c>
       <c r="C146" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D146" t="s">
         <v>47</v>
@@ -4307,7 +4307,7 @@
         <v>224</v>
       </c>
       <c r="C147" t="s">
-        <v>231</v>
+        <v>322</v>
       </c>
       <c r="D147" t="s">
         <v>47</v>
@@ -4330,8 +4330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0E4DC4-ABC2-455B-9DCE-7C09A6B70159}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4386,42 +4386,42 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B8" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B9" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B11" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>